<commit_message>
table of effort and proportion undersize
</commit_message>
<xml_diff>
--- a/docs/Data/TyeeCatchData.xlsx
+++ b/docs/Data/TyeeCatchData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evogt\R Analysis\EAV\GitHubMarkdown\R-Markdown-GitHub-Page\docs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECB863C-9544-42DB-81B1-FF2552E184F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4B4141-F67D-4FBF-A7FD-6F4ADF83A14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54135" yWindow="870" windowWidth="21270" windowHeight="11460" xr2:uid="{0CB3CDF9-0205-43C4-ADC8-DEC6E991EEB1}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0CB3CDF9-0205-43C4-ADC8-DEC6E991EEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="20">
   <si>
     <t>Year</t>
   </si>
@@ -118,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,11 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99EFA95-E1A2-4F3D-8001-3428518B60BC}">
-  <dimension ref="A1:J720"/>
+  <dimension ref="A1:J723"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A708" workbookViewId="0">
-      <selection activeCell="J720" sqref="J720"/>
+    <sheetView tabSelected="1" topLeftCell="A705" workbookViewId="0">
+      <selection activeCell="E725" sqref="E725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23142,7 +23150,7 @@
         <v>0.25</v>
       </c>
       <c r="I704" s="3">
-        <f t="shared" ref="I704:I719" si="11">C704+H704</f>
+        <f t="shared" ref="I704:I721" si="11">C704+H704</f>
         <v>44787.25</v>
       </c>
       <c r="J704" t="s">
@@ -23649,7 +23657,106 @@
       </c>
     </row>
     <row r="720" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I720" s="3"/>
+      <c r="A720">
+        <v>2023</v>
+      </c>
+      <c r="B720">
+        <v>2</v>
+      </c>
+      <c r="C720" s="1">
+        <v>45158</v>
+      </c>
+      <c r="D720" s="1">
+        <v>44793</v>
+      </c>
+      <c r="E720">
+        <v>31.14</v>
+      </c>
+      <c r="F720" t="s">
+        <v>5</v>
+      </c>
+      <c r="G720" s="2">
+        <v>0.87986111111111109</v>
+      </c>
+      <c r="H720" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="I720" s="3">
+        <f t="shared" si="11"/>
+        <v>45158.875</v>
+      </c>
+      <c r="J720" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="721" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A721">
+        <v>2023</v>
+      </c>
+      <c r="B721">
+        <v>2</v>
+      </c>
+      <c r="C721" s="1">
+        <v>45159</v>
+      </c>
+      <c r="D721" s="1">
+        <v>44794</v>
+      </c>
+      <c r="E721" s="4">
+        <v>40.696969000000003</v>
+      </c>
+      <c r="F721" t="s">
+        <v>5</v>
+      </c>
+      <c r="G721" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="H721" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="I721" s="3">
+        <f t="shared" si="11"/>
+        <v>45159.875</v>
+      </c>
+      <c r="J721" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="722" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A722">
+        <v>2023</v>
+      </c>
+      <c r="B722">
+        <v>2</v>
+      </c>
+      <c r="C722" s="1">
+        <v>45159</v>
+      </c>
+      <c r="D722" s="1">
+        <v>44794</v>
+      </c>
+      <c r="E722" s="4">
+        <v>30.696968999999999</v>
+      </c>
+      <c r="F722" t="s">
+        <v>5</v>
+      </c>
+      <c r="G722" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="H722" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="I722" s="3">
+        <f t="shared" ref="I722" si="13">C722+H722</f>
+        <v>45159.875</v>
+      </c>
+      <c r="J722" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="723" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I723" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J708" xr:uid="{A99EFA95-E1A2-4F3D-8001-3428518B60BC}"/>

</xml_diff>

<commit_message>
added catch and release mortality section and removed scribbles
</commit_message>
<xml_diff>
--- a/docs/Data/TyeeCatchData.xlsx
+++ b/docs/Data/TyeeCatchData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evogt\R Analysis\EAV\GitHubMarkdown\R-Markdown-GitHub-Page\docs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA56742A-B466-477E-9FFD-6687F9DB3CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A559A8-6D1D-463F-AD73-6EE1187EE38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CB3CDF9-0205-43C4-ADC8-DEC6E991EEB1}"/>
+    <workbookView xWindow="-26025" yWindow="2235" windowWidth="21600" windowHeight="11235" xr2:uid="{0CB3CDF9-0205-43C4-ADC8-DEC6E991EEB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4301" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4313" uniqueCount="559">
   <si>
     <t>Year</t>
   </si>
@@ -1712,6 +1712,9 @@
   </si>
   <si>
     <t>Allyn Harvey</t>
+  </si>
+  <si>
+    <t>John Plant</t>
   </si>
 </sst>
 </file>
@@ -2081,13 +2084,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99EFA95-E1A2-4F3D-8001-3428518B60BC}">
-  <dimension ref="A1:O731"/>
+  <dimension ref="A1:O733"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D714" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D729" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O730" sqref="O730"/>
+      <selection pane="bottomRight" activeCell="L726" sqref="B726:L727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37347,7 +37350,7 @@
         <v>0.25</v>
       </c>
       <c r="J731" s="7">
-        <f t="shared" ref="J731" si="26">D731+I731</f>
+        <f t="shared" ref="J731:J732" si="26">D731+I731</f>
         <v>45165.25</v>
       </c>
       <c r="K731" t="s">
@@ -37363,6 +37366,102 @@
         <v>24</v>
       </c>
       <c r="O731" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="732" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A732">
+        <v>2023</v>
+      </c>
+      <c r="B732">
+        <v>2</v>
+      </c>
+      <c r="C732">
+        <v>23</v>
+      </c>
+      <c r="D732" s="1">
+        <v>45167</v>
+      </c>
+      <c r="E732" s="1">
+        <v>44802</v>
+      </c>
+      <c r="F732" s="5">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="G732" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H732" s="2">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="I732" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J732" s="7">
+        <f t="shared" si="26"/>
+        <v>45167.833333333336</v>
+      </c>
+      <c r="K732" t="s">
+        <v>8</v>
+      </c>
+      <c r="L732" t="s">
+        <v>558</v>
+      </c>
+      <c r="M732" t="s">
+        <v>276</v>
+      </c>
+      <c r="N732" t="s">
+        <v>127</v>
+      </c>
+      <c r="O732" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="733" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A733">
+        <v>2023</v>
+      </c>
+      <c r="B733">
+        <v>2</v>
+      </c>
+      <c r="C733">
+        <v>24</v>
+      </c>
+      <c r="D733" s="1">
+        <v>45167</v>
+      </c>
+      <c r="E733" s="1">
+        <v>44803</v>
+      </c>
+      <c r="F733" s="5">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="G733" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H733" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="I733" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J733" s="7">
+        <f t="shared" ref="J733" si="27">D733+I733</f>
+        <v>45167.416666666664</v>
+      </c>
+      <c r="K733" t="s">
+        <v>6</v>
+      </c>
+      <c r="L733" t="s">
+        <v>495</v>
+      </c>
+      <c r="M733" t="s">
+        <v>216</v>
+      </c>
+      <c r="N733" t="s">
+        <v>127</v>
+      </c>
+      <c r="O733" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>